<commit_message>
year col bug fix
</commit_message>
<xml_diff>
--- a/data/xvariables-final.xlsx
+++ b/data/xvariables-final.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="xvariables" sheetId="1" r:id="rId1"/>
@@ -9299,8 +9299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2720"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1539" workbookViewId="0">
-      <selection activeCell="B1561" sqref="B1561"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9371,6 +9371,9 @@
         <v>2712</v>
       </c>
       <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>0</v>
       </c>
     </row>

</xml_diff>